<commit_message>
Add Scene Availbility calculation
</commit_message>
<xml_diff>
--- a/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
+++ b/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="192">
   <si>
     <t xml:space="preserve">KPI ID</t>
   </si>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">B2</t>
   </si>
   <si>
-    <t xml:space="preserve">Does the End Cap Include Coca-Cola .5L 6 Pack? </t>
+    <t xml:space="preserve">Does the End Cap Include Coca-Cola .5L 6 Pack?</t>
   </si>
   <si>
     <t xml:space="preserve">If Yes, does the end cap include 6pk .5L Coca-Cola</t>
@@ -878,17 +878,18 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.0037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="95.1518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.0222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="99.9555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -967,7 +968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1311,34 +1312,35 @@
   </sheetPr>
   <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.0518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="72.3185185185185"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="29.4"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="43.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.7962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="75.9444444444444"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="45.4703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2070,7 +2072,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>51</v>
       </c>
@@ -2106,7 +2108,9 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="R9" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="S9" s="4" t="n">
         <v>1</v>
       </c>
@@ -2467,21 +2471,25 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.2185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="44.5888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.6962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.0777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="46.8407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,22 +2877,26 @@
   </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.6333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="78.5925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.2592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.5111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.2814814814815"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3081,20 +3093,23 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.9777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.6555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.7925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.38148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.74814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.8518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update Facings SOS calculation
</commit_message>
<xml_diff>
--- a/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
+++ b/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="191">
   <si>
     <t xml:space="preserve">KPI ID</t>
   </si>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">O1</t>
   </si>
   <si>
-    <t xml:space="preserve">SOVI Main Beverage Aisle </t>
+    <t xml:space="preserve">SOVI Main Beverage Aisle</t>
   </si>
   <si>
     <t xml:space="preserve">SOVI Main Bev Aisle Manufacturer within Category</t>
@@ -371,7 +371,7 @@
     <t xml:space="preserve">CCNA</t>
   </si>
   <si>
-    <t xml:space="preserve">Key Package</t>
+    <t xml:space="preserve">KEY PACKAGE</t>
   </si>
   <si>
     <t xml:space="preserve">12OZ 24PK CAN</t>
@@ -548,18 +548,21 @@
     <t xml:space="preserve">[A] facings / [B] facings &gt;50% COUNT BAY</t>
   </si>
   <si>
+    <t xml:space="preserve">M - Beverage Aisle/Shelf - All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCNA,FAIRLIFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
     <t xml:space="preserve">M - Coolers at Main Checkout</t>
   </si>
   <si>
-    <t xml:space="preserve">1,1802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCNA,FAIRLIFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculation</t>
-  </si>
-  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
@@ -569,7 +572,7 @@
     <t xml:space="preserve">1,1802,4</t>
   </si>
   <si>
-    <t xml:space="preserve">CCNA.FAIRLIFE,PBNA</t>
+    <t xml:space="preserve">CCNA,FAIRLIFE,PBNA</t>
   </si>
   <si>
     <t xml:space="preserve">M - Coolers at Self Check-Out</t>
@@ -578,43 +581,37 @@
     <t xml:space="preserve">Context Entity</t>
   </si>
   <si>
-    <t xml:space="preserve">M - Beverage Aisle/Shelf - All (Separated by Category)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturer</t>
+    <t xml:space="preserve">product_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU,Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufcaturer</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU,Empty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a_facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufcaturer</t>
   </si>
 </sst>
 </file>
@@ -878,18 +875,18 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.0222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="99.9555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.6444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="110.633333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1204,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -1312,35 +1309,33 @@
   </sheetPr>
   <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C18 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="75.9444444444444"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="30.8666666666667"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.6222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="64.9703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.7481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="83.8814814814815"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="50.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2471,25 +2466,26 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="C18 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.6962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.0777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="46.8407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.3592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="51.6444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.5037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2546,7 @@
       <c r="Y1" s="10"/>
       <c r="Z1" s="10"/>
     </row>
-    <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -2602,7 +2598,7 @@
       <c r="Y2" s="10"/>
       <c r="Z2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -2619,16 +2615,16 @@
         <v>168</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>113</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2653,7 +2649,7 @@
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -2670,7 +2666,7 @@
         <v>168</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G4" s="4"/>
       <c r="I4" s="4"/>
@@ -2678,10 +2674,10 @@
         <v>113</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>172</v>
@@ -2704,7 +2700,7 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -2721,7 +2717,7 @@
         <v>168</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>113</v>
@@ -2756,7 +2752,7 @@
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -2773,16 +2769,16 @@
         <v>168</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>113</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -2807,7 +2803,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -2824,7 +2820,7 @@
         <v>168</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -2833,10 +2829,10 @@
         <v>113</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>172</v>
@@ -2877,26 +2873,26 @@
   </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C18 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.2592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.5111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="39.2962962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.2814814814815"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.2962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="91.1333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.3925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="43.3148148148148"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.3185185185185"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2922,7 +2918,7 @@
         <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>78</v>
@@ -2946,7 +2942,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2960,38 +2956,38 @@
         <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="30.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -3005,40 +3001,40 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="30.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>67</v>
       </c>
@@ -3049,30 +3045,38 @@
         <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="M4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3093,23 +3097,23 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C18 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.38148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.74814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.67037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.8518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2925925925926"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.3074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,13 +3139,13 @@
         <v>107</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3161,10 +3165,10 @@
         <v>162</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>108</v>
@@ -3173,7 +3177,7 @@
         <v>109</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duplicate CCUS and wrap load_session_data() in try-except block
</commit_message>
<xml_diff>
--- a/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
+++ b/Projects/CCUS_SAND2/MILITARY/Data/CCUS_Military_06112020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="190">
   <si>
     <t xml:space="preserve">KPI ID</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">SOVI Displays (all scenes) Manufacturer within Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facings SOS</t>
   </si>
   <si>
     <t xml:space="preserve">S1</t>
@@ -402,7 +399,7 @@
 (failed scenes should not have a result)</t>
   </si>
   <si>
-    <t xml:space="preserve">location</t>
+    <t xml:space="preserve">location_fk</t>
   </si>
   <si>
     <t xml:space="preserve">store_task_area_group_item_fk</t>
@@ -548,7 +545,7 @@
     <t xml:space="preserve">[A] facings / [B] facings &gt;50% COUNT BAY</t>
   </si>
   <si>
-    <t xml:space="preserve">M - Beverage Aisle/Shelf - All</t>
+    <t xml:space="preserve">M - Beverage Aisle/Shelf - All </t>
   </si>
   <si>
     <t xml:space="preserve">1,1802</t>
@@ -875,18 +872,18 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.6444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="110.633333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="84.6666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1255,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -1267,7 +1264,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>10</v>
@@ -1275,17 +1272,17 @@
     </row>
     <row r="22" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>10</v>
@@ -1309,33 +1306,35 @@
   </sheetPr>
   <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C18 A3"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="AH1" activeCellId="0" sqref="AH1"/>
+      <selection pane="bottomLeft" activeCell="AL4" activeCellId="0" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.6222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="64.9703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.7481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="83.8814814814815"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="50.0740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.5925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.5481481481482"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="32.2407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="95.0555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="18" min="14" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="34" min="19" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="56.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1355,112 +1354,112 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,33 +1477,33 @@
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S2" s="4" t="n">
         <v>3</v>
@@ -1530,25 +1529,25 @@
         <v>172</v>
       </c>
       <c r="AJ2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AN2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="101.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1565,36 +1564,36 @@
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S3" s="4" t="n">
         <v>3</v>
@@ -1618,19 +1617,19 @@
         <v>172</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="AL3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM3" s="7" t="s">
+      <c r="AN3" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="AN3" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="AO3" s="8" t="n">
         <v>1</v>
@@ -1651,17 +1650,17 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="K4" s="4" t="n">
         <v>6</v>
@@ -1673,7 +1672,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S4" s="4" t="n">
         <v>1</v>
@@ -1698,19 +1697,19 @@
       <c r="AI4" s="9"/>
       <c r="AJ4" s="9"/>
       <c r="AK4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL4" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AM4" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM4" s="6" t="s">
+      <c r="AN4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1730,17 +1729,17 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="K5" s="4" t="n">
         <v>6</v>
@@ -1752,16 +1751,16 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="T5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="V5" s="4" t="n">
         <v>22</v>
@@ -1769,10 +1768,10 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA5" s="4" t="n">
         <v>1</v>
@@ -1787,19 +1786,19 @@
       <c r="AI5" s="9"/>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AM5" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM5" s="6" t="s">
+      <c r="AN5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO5" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,17 +1816,17 @@
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K6" s="4" t="n">
         <v>90</v>
@@ -1839,7 +1838,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S6" s="4" t="n">
         <v>6</v>
@@ -1863,22 +1862,22 @@
         <v>172</v>
       </c>
       <c r="AJ6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK6" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AK6" s="4" t="s">
+      <c r="AL6" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL6" s="4" t="s">
+      <c r="AM6" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM6" s="6" t="s">
+      <c r="AN6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="115.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,48 +1895,48 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="Q7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S7" s="4" t="n">
         <v>4</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V7" s="4" t="n">
         <v>35</v>
@@ -1945,10 +1944,10 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA7" s="4" t="n">
         <v>1</v>
@@ -1966,22 +1965,22 @@
         <v>172</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL7" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL7" s="4" t="s">
+      <c r="AM7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM7" s="6" t="s">
+      <c r="AN7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO7" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1999,23 +1998,23 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="K8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="n">
@@ -2025,7 +2024,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S8" s="4" t="n">
         <v>5</v>
@@ -2049,22 +2048,22 @@
         <v>172</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL8" s="4" t="s">
+      <c r="AM8" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM8" s="6" t="s">
+      <c r="AN8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO8" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,20 +2081,20 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
@@ -2104,27 +2103,27 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S9" s="4" t="n">
         <v>1</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="V9" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Z9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA9" s="4" t="n">
         <v>1</v>
@@ -2142,22 +2141,22 @@
         <v>172</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL9" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL9" s="4" t="s">
+      <c r="AM9" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM9" s="6" t="s">
+      <c r="AN9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,20 +2174,20 @@
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -2197,7 +2196,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S10" s="4" t="n">
         <v>6</v>
@@ -2223,22 +2222,22 @@
         <v>172</v>
       </c>
       <c r="AJ10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK10" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AL10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL10" s="4" t="s">
+      <c r="AM10" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM10" s="6" t="s">
+      <c r="AN10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,20 +2255,20 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -2278,52 +2277,52 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S11" s="4" t="n">
         <v>7</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="V11" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="W11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="X11" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="W11" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="Y11" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AA11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AD11" s="6" t="s">
+      <c r="AE11" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="AE11" s="6" t="s">
+      <c r="AF11" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG11" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="AF11" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG11" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="AH11" s="4" t="n">
         <v>1</v>
@@ -2332,22 +2331,22 @@
         <v>172</v>
       </c>
       <c r="AJ11" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL11" s="4" t="s">
+      <c r="AM11" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM11" s="6" t="s">
+      <c r="AN11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO11" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="72.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,54 +2365,54 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S12" s="4" t="n">
         <v>216</v>
       </c>
       <c r="T12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="U12" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="V12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W12" s="4" t="s">
+      <c r="X12" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="Y12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z12" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="AA12" s="4" t="n">
         <v>108</v>
@@ -2430,19 +2429,19 @@
       <c r="AI12" s="9"/>
       <c r="AJ12" s="9"/>
       <c r="AK12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL12" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL12" s="4" t="s">
+      <c r="AM12" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AM12" s="6" t="s">
+      <c r="AN12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="AN12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,26 +2465,27 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="C18 F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.3592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="51.6444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.637037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.6703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.6148148148148"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,37 +2502,37 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -2546,7 +2546,7 @@
       <c r="Y1" s="10"/>
       <c r="Z1" s="10"/>
     </row>
-    <row r="2" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -2560,31 +2560,31 @@
         <v>35</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
@@ -2612,30 +2612,30 @@
         <v>35</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
@@ -2663,30 +2663,30 @@
         <v>35</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>177</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -2714,31 +2714,31 @@
         <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -2766,30 +2766,30 @@
         <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -2803,7 +2803,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="44.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="30.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -2817,31 +2817,31 @@
         <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="9"/>
       <c r="J7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>177</v>
-      </c>
       <c r="M7" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
@@ -2874,25 +2874,25 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C18 B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.2962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="91.1333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.3925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="43.3148148148148"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.3185185185185"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.562962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="103.188888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.0740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="48.9"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="37.6296296296296"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2909,40 +2909,40 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2956,38 +2956,38 @@
         <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -3001,37 +3001,37 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3048,35 +3048,35 @@
         <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3098,22 +3098,22 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C18 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.3074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.0481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.4222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,54 +3130,54 @@
         <v>4</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>107</v>
-      </c>
       <c r="H1" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>